<commit_message>
Update database structure and entries
</commit_message>
<xml_diff>
--- a/Kassitische_Personen_Namen.xlsx
+++ b/Kassitische_Personen_Namen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahschier/kassitisch_db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25408CC0-B781-D44A-997E-6CD0AF894D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A25B337-72F6-D74A-8682-DB048A5F4131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kassitische Analyse" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="434">
   <si>
     <t>Name</t>
   </si>
@@ -1048,6 +1048,285 @@
   </si>
   <si>
     <t>Uz-ub</t>
+  </si>
+  <si>
+    <t>Abi-Rataš</t>
+  </si>
+  <si>
+    <t>Abi-Rutaš</t>
+  </si>
+  <si>
+    <t>Agum</t>
+  </si>
+  <si>
+    <t>Alba-da</t>
+  </si>
+  <si>
+    <t>Albadi-Saḫ</t>
+  </si>
+  <si>
+    <t>Ališbi-Saḫ</t>
+  </si>
+  <si>
+    <t>Ailzibu</t>
+  </si>
+  <si>
+    <t>Alzibu-naša</t>
+  </si>
+  <si>
+    <t>Alsa-duri</t>
+  </si>
+  <si>
+    <t>Ašar-Saḫ</t>
+  </si>
+  <si>
+    <t>Ani-kilamdi</t>
+  </si>
+  <si>
+    <t>Ašriqu</t>
+  </si>
+  <si>
+    <t>Badu-Zana</t>
+  </si>
+  <si>
+    <t>Bi-Bugašu</t>
+  </si>
+  <si>
+    <t>Biri-šuriyaš</t>
+  </si>
+  <si>
+    <t>Bula-ḫali</t>
+  </si>
+  <si>
+    <t>bula-nikir</t>
+  </si>
+  <si>
+    <t>Bunabu</t>
+  </si>
+  <si>
+    <t>Bunnie</t>
+  </si>
+  <si>
+    <t>Bunni-ḫarpa</t>
+  </si>
+  <si>
+    <t>Bunni-tura</t>
+  </si>
+  <si>
+    <t>Buramizi</t>
+  </si>
+  <si>
+    <t>Bura-saḫ</t>
+  </si>
+  <si>
+    <t>Bura-Sana</t>
+  </si>
+  <si>
+    <t>Buraša-Marduk</t>
+  </si>
+  <si>
+    <t>Bureya</t>
+  </si>
+  <si>
+    <t>Burna-Adad</t>
+  </si>
+  <si>
+    <t>Burnami-saḫ</t>
+  </si>
+  <si>
+    <t>burna-Harbašu</t>
+  </si>
+  <si>
+    <t>Burnabiḫe</t>
+  </si>
+  <si>
+    <t>burnabu</t>
+  </si>
+  <si>
+    <t>Burna-zini</t>
+  </si>
+  <si>
+    <t>burni</t>
+  </si>
+  <si>
+    <t>burni-durum</t>
+  </si>
+  <si>
+    <t>burni-dura</t>
+  </si>
+  <si>
+    <t>burni-mašḫu</t>
+  </si>
+  <si>
+    <t>burpa-suqšu</t>
+  </si>
+  <si>
+    <t>Burra-alban</t>
+  </si>
+  <si>
+    <t>burra-laguda</t>
+  </si>
+  <si>
+    <t>burraši-galdu</t>
+  </si>
+  <si>
+    <t>burra-šikme</t>
+  </si>
+  <si>
+    <t>burra-šuḫur</t>
+  </si>
+  <si>
+    <t>burra-šuqamuna</t>
+  </si>
+  <si>
+    <t>burra-turra</t>
+  </si>
+  <si>
+    <t>burra-akmul</t>
+  </si>
+  <si>
+    <t>burrutu</t>
+  </si>
+  <si>
+    <t>duni-mašḫu</t>
+  </si>
+  <si>
+    <t>ebi-rattaš</t>
+  </si>
+  <si>
+    <t>gab-buriyaš</t>
+  </si>
+  <si>
+    <t>gab-ḫarbe</t>
+  </si>
+  <si>
+    <t>gab-satran</t>
+  </si>
+  <si>
+    <t>gab-šuqamuna</t>
+  </si>
+  <si>
+    <t>gaddaš</t>
+  </si>
+  <si>
+    <t>gandaš</t>
+  </si>
+  <si>
+    <t>gandi</t>
+  </si>
+  <si>
+    <t>gerza-bura</t>
+  </si>
+  <si>
+    <t>kirza-bura</t>
+  </si>
+  <si>
+    <t>gunini-bugaš</t>
+  </si>
+  <si>
+    <t>gunizar-bugaš</t>
+  </si>
+  <si>
+    <t>gurba-saḫ</t>
+  </si>
+  <si>
+    <t>gurpazaduya</t>
+  </si>
+  <si>
+    <t>guzalzal-bugaš</t>
+  </si>
+  <si>
+    <t>guzar-ali</t>
+  </si>
+  <si>
+    <t>guzaru</t>
+  </si>
+  <si>
+    <t>ḫamaš-šarri</t>
+  </si>
+  <si>
+    <t>ḫamaš-šuk</t>
+  </si>
+  <si>
+    <t>ḫāmaš-šugab</t>
+  </si>
+  <si>
+    <t>ḫārbal-saḫ</t>
+  </si>
+  <si>
+    <t>ḫarpaniwe</t>
+  </si>
+  <si>
+    <t>ḫarba-šiḫu</t>
+  </si>
+  <si>
+    <t>ḫašardu</t>
+  </si>
+  <si>
+    <t>ḫašmar-galšu</t>
+  </si>
+  <si>
+    <t>ḫašuar</t>
+  </si>
+  <si>
+    <t>ḫirzi</t>
+  </si>
+  <si>
+    <t>ḫudi-yazi</t>
+  </si>
+  <si>
+    <t>ḫumurbi</t>
+  </si>
+  <si>
+    <t>ḫumurti</t>
+  </si>
+  <si>
+    <t>ḫuri-saḫ</t>
+  </si>
+  <si>
+    <t>ḫušši-ḫarbe</t>
+  </si>
+  <si>
+    <t>ḫuštiya</t>
+  </si>
+  <si>
+    <t>Ibša-ḫalu</t>
+  </si>
+  <si>
+    <t>ibša</t>
+  </si>
+  <si>
+    <t>ili-šarigaš</t>
+  </si>
+  <si>
+    <t>inza-ḫudak</t>
+  </si>
+  <si>
+    <t>inzatum</t>
+  </si>
+  <si>
+    <t>inzi-mašḫu</t>
+  </si>
+  <si>
+    <t>inzite</t>
+  </si>
+  <si>
+    <t>inzi-tešup</t>
+  </si>
+  <si>
+    <t>inzu</t>
+  </si>
+  <si>
+    <t>ibzu-ḫusieš</t>
+  </si>
+  <si>
+    <t>inzu-kutir</t>
+  </si>
+  <si>
+    <t>inzu-mena</t>
+  </si>
+  <si>
+    <t>inzu-murudaš</t>
   </si>
 </sst>
 </file>
@@ -1065,11 +1344,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1315,11 +1596,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E191"/>
+  <dimension ref="A1:E287"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="291" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C280" sqref="C280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3141,6 +3422,486 @@
         <v>340</v>
       </c>
     </row>
+    <row r="192" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A205" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A208" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A209" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A210" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A212" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A214" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A215" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A216" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A217" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A218" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A219" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A220" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A221" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A222" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A223" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A224" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A225" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A226" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A227" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A228" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A229" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A230" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A231" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A232" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A233" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A234" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A235" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A236" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A237" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A238" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A239" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A241" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A242" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A243" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A244" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A245" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A246" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A247" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A248" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A249" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A250" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A251" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A252" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A253" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A254" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A255" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A256" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A257" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A258" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A259" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A260" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A261" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A262" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A263" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A264" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A265" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A266" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A267" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A268" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A269" s="1" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A270" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A271" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A272" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A273" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A274" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A275" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A276" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A277" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A278" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A279" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A280" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A281" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A282" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A283" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A284" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A285" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A286" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A287" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>